<commit_message>
Consistency in name across different types
</commit_message>
<xml_diff>
--- a/utils/document/types.xlsx
+++ b/utils/document/types.xlsx
@@ -25,25 +25,25 @@
     <t>providerItem</t>
   </si>
   <si>
-    <t>id, providerName, tags, refBaseSchema, itemDescription, itemType</t>
+    <t xml:space="preserve">id, providerName(name), tags, refBaseSchema, itemDescription, itemType, </t>
   </si>
   <si>
     <t>resourceItem</t>
   </si>
   <si>
-    <t>id, tags, refBaseSchema, resourceServer, itemDescription, refDataModel, provider, resourceServerGroup, resourceId, itemType</t>
+    <t xml:space="preserve">id, tags, refBaseSchema, resourceServer, itemDescription, refDataModel, provider, resourceServerGroup, resourceId, itemType, </t>
   </si>
   <si>
     <t>resourceServer</t>
   </si>
   <si>
-    <t>id, name, tags, refBaseSchema, itemDescription, resourceServerHTTPAccessURL, resourceServerOrg, resourceServerGroups, coverageRegion, itemType</t>
+    <t xml:space="preserve">id, name, tags, refBaseSchema, itemDescription, resourceServerHTTPAccessURL(uriLink), resourceServerOrg(organizationInfo), coverageRegion, itemType, </t>
   </si>
   <si>
     <t>resourceServerGroup</t>
   </si>
   <si>
-    <t>id, name, tags, refBaseSchema, resourceServer, itemDescription, refDataModel, provider, itemType</t>
+    <t xml:space="preserve">id, name, tags, refBaseSchema, resourceServer, itemDescription, refDataModel, provider, itemType, </t>
   </si>
 </sst>
 </file>
@@ -67,6 +67,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>

</xml_diff>